<commit_message>
Round formula results to 2 decimal places
Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Presets.xlsx
+++ b/Presets.xlsx
@@ -155,19 +155,19 @@
         <ns0:v>0.34</ns0:v>
       </ns0:c>
       <ns0:c r="C5" s="0">
-        <ns0:f>B5*C$3</ns0:f>
+        <ns0:f>ROUND(B5*C$3,2)</ns0:f>
       </ns0:c>
       <ns0:c r="D5" s="0">
-        <ns0:f>B5*D$3</ns0:f>
+        <ns0:f>ROUND(B5*D$3,2)</ns0:f>
       </ns0:c>
       <ns0:c r="E5" s="0">
-        <ns0:f>B5*E$3</ns0:f>
+        <ns0:f>ROUND(B5*E$3,2)</ns0:f>
       </ns0:c>
       <ns0:c r="F5" s="0">
-        <ns0:f>B5*F$3</ns0:f>
+        <ns0:f>ROUND(B5*F$3,2)</ns0:f>
       </ns0:c>
       <ns0:c r="G5" s="0">
-        <ns0:f>B5*G$3</ns0:f>
+        <ns0:f>ROUND(B5*G$3,2)</ns0:f>
       </ns0:c>
     </ns0:row>
     <ns0:row r="6">
@@ -180,19 +180,19 @@
         <ns0:v>0.3</ns0:v>
       </ns0:c>
       <ns0:c r="C6" s="0">
-        <ns0:f>B6*C$3</ns0:f>
+        <ns0:f>ROUND(B6*C$3,2)</ns0:f>
       </ns0:c>
       <ns0:c r="D6" s="0">
-        <ns0:f>B6*D$3</ns0:f>
+        <ns0:f>ROUND(B6*D$3,2)</ns0:f>
       </ns0:c>
       <ns0:c r="E6" s="0">
-        <ns0:f>B6*E$3</ns0:f>
+        <ns0:f>ROUND(B6*E$3,2)</ns0:f>
       </ns0:c>
       <ns0:c r="F6" s="0">
-        <ns0:f>B6*F$3</ns0:f>
+        <ns0:f>ROUND(B6*F$3,2)</ns0:f>
       </ns0:c>
       <ns0:c r="G6" s="0">
-        <ns0:f>B6*G$3</ns0:f>
+        <ns0:f>ROUND(B6*G$3,2)</ns0:f>
       </ns0:c>
     </ns0:row>
     <ns0:row r="7">
@@ -205,19 +205,19 @@
         <ns0:v>0.28</ns0:v>
       </ns0:c>
       <ns0:c r="C7" s="0">
-        <ns0:f>B7*C$3</ns0:f>
+        <ns0:f>ROUND(B7*C$3,2)</ns0:f>
       </ns0:c>
       <ns0:c r="D7" s="0">
-        <ns0:f>B7*D$3</ns0:f>
+        <ns0:f>ROUND(B7*D$3,2)</ns0:f>
       </ns0:c>
       <ns0:c r="E7" s="0">
-        <ns0:f>B7*E$3</ns0:f>
+        <ns0:f>ROUND(B7*E$3,2)</ns0:f>
       </ns0:c>
       <ns0:c r="F7" s="0">
-        <ns0:f>B7*F$3</ns0:f>
+        <ns0:f>ROUND(B7*F$3,2)</ns0:f>
       </ns0:c>
       <ns0:c r="G7" s="0">
-        <ns0:f>B7*G$3</ns0:f>
+        <ns0:f>ROUND(B7*G$3,2)</ns0:f>
       </ns0:c>
     </ns0:row>
     <ns0:row r="8">
@@ -230,19 +230,19 @@
         <ns0:v>0.26</ns0:v>
       </ns0:c>
       <ns0:c r="C8" s="0">
-        <ns0:f>B8*C$3</ns0:f>
+        <ns0:f>ROUND(B8*C$3,2)</ns0:f>
       </ns0:c>
       <ns0:c r="D8" s="0">
-        <ns0:f>B8*D$3</ns0:f>
+        <ns0:f>ROUND(B8*D$3,2)</ns0:f>
       </ns0:c>
       <ns0:c r="E8" s="0">
-        <ns0:f>B8*E$3</ns0:f>
+        <ns0:f>ROUND(B8*E$3,2)</ns0:f>
       </ns0:c>
       <ns0:c r="F8" s="0">
-        <ns0:f>B8*F$3</ns0:f>
+        <ns0:f>ROUND(B8*F$3,2)</ns0:f>
       </ns0:c>
       <ns0:c r="G8" s="0">
-        <ns0:f>B8*G$3</ns0:f>
+        <ns0:f>ROUND(B8*G$3,2)</ns0:f>
       </ns0:c>
     </ns0:row>
     <ns0:row r="9">
@@ -255,19 +255,19 @@
         <ns0:v>0.25</ns0:v>
       </ns0:c>
       <ns0:c r="C9" s="0">
-        <ns0:f>B9*C$3</ns0:f>
+        <ns0:f>ROUND(B9*C$3,2)</ns0:f>
       </ns0:c>
       <ns0:c r="D9" s="0">
-        <ns0:f>B9*D$3</ns0:f>
+        <ns0:f>ROUND(B9*D$3,2)</ns0:f>
       </ns0:c>
       <ns0:c r="E9" s="0">
-        <ns0:f>B9*E$3</ns0:f>
+        <ns0:f>ROUND(B9*E$3,2)</ns0:f>
       </ns0:c>
       <ns0:c r="F9" s="0">
-        <ns0:f>B9*F$3</ns0:f>
+        <ns0:f>ROUND(B9*F$3,2)</ns0:f>
       </ns0:c>
       <ns0:c r="G9" s="0">
-        <ns0:f>B9*G$3</ns0:f>
+        <ns0:f>ROUND(B9*G$3,2)</ns0:f>
       </ns0:c>
     </ns0:row>
     <ns0:row r="10">
@@ -280,19 +280,19 @@
         <ns0:v>0.23</ns0:v>
       </ns0:c>
       <ns0:c r="C10" s="0">
-        <ns0:f>B10*C$3</ns0:f>
+        <ns0:f>ROUND(B10*C$3,2)</ns0:f>
       </ns0:c>
       <ns0:c r="D10" s="0">
-        <ns0:f>B10*D$3</ns0:f>
+        <ns0:f>ROUND(B10*D$3,2)</ns0:f>
       </ns0:c>
       <ns0:c r="E10" s="0">
-        <ns0:f>B10*E$3</ns0:f>
+        <ns0:f>ROUND(B10*E$3,2)</ns0:f>
       </ns0:c>
       <ns0:c r="F10" s="0">
-        <ns0:f>B10*F$3</ns0:f>
+        <ns0:f>ROUND(B10*F$3,2)</ns0:f>
       </ns0:c>
       <ns0:c r="G10" s="0">
-        <ns0:f>B10*G$3</ns0:f>
+        <ns0:f>ROUND(B10*G$3,2)</ns0:f>
       </ns0:c>
     </ns0:row>
     <ns0:row r="11">
@@ -305,19 +305,19 @@
         <ns0:v>0.21</ns0:v>
       </ns0:c>
       <ns0:c r="C11" s="0">
-        <ns0:f>B11*C$3</ns0:f>
+        <ns0:f>ROUND(B11*C$3,2)</ns0:f>
       </ns0:c>
       <ns0:c r="D11" s="0">
-        <ns0:f>B11*D$3</ns0:f>
+        <ns0:f>ROUND(B11*D$3,2)</ns0:f>
       </ns0:c>
       <ns0:c r="E11" s="0">
-        <ns0:f>B11*E$3</ns0:f>
+        <ns0:f>ROUND(B11*E$3,2)</ns0:f>
       </ns0:c>
       <ns0:c r="F11" s="0">
-        <ns0:f>B11*F$3</ns0:f>
+        <ns0:f>ROUND(B11*F$3,2)</ns0:f>
       </ns0:c>
       <ns0:c r="G11" s="0">
-        <ns0:f>B11*G$3</ns0:f>
+        <ns0:f>ROUND(B11*G$3,2)</ns0:f>
       </ns0:c>
     </ns0:row>
     <ns0:row r="12"/>
@@ -394,19 +394,19 @@
         <ns0:v>1.5</ns0:v>
       </ns0:c>
       <ns0:c r="C18" s="0">
-        <ns0:f>B18*C$16</ns0:f>
+        <ns0:f>ROUND(B18*C$16,2)</ns0:f>
       </ns0:c>
       <ns0:c r="D18" s="0">
-        <ns0:f>B18*D$16</ns0:f>
+        <ns0:f>ROUND(B18*D$16,2)</ns0:f>
       </ns0:c>
       <ns0:c r="E18" s="0">
-        <ns0:f>B18*E$16</ns0:f>
+        <ns0:f>ROUND(B18*E$16,2)</ns0:f>
       </ns0:c>
       <ns0:c r="F18" s="0">
-        <ns0:f>B18*F$16</ns0:f>
+        <ns0:f>ROUND(B18*F$16,2)</ns0:f>
       </ns0:c>
       <ns0:c r="G18" s="0">
-        <ns0:f>B18*G$16</ns0:f>
+        <ns0:f>ROUND(B18*G$16,2)</ns0:f>
       </ns0:c>
     </ns0:row>
     <ns0:row r="19">
@@ -419,19 +419,19 @@
         <ns0:v>2.0</ns0:v>
       </ns0:c>
       <ns0:c r="C19" s="0">
-        <ns0:f>B19*C$16</ns0:f>
+        <ns0:f>ROUND(B19*C$16,2)</ns0:f>
       </ns0:c>
       <ns0:c r="D19" s="0">
-        <ns0:f>B19*D$16</ns0:f>
+        <ns0:f>ROUND(B19*D$16,2)</ns0:f>
       </ns0:c>
       <ns0:c r="E19" s="0">
-        <ns0:f>B19*E$16</ns0:f>
+        <ns0:f>ROUND(B19*E$16,2)</ns0:f>
       </ns0:c>
       <ns0:c r="F19" s="0">
-        <ns0:f>B19*F$16</ns0:f>
+        <ns0:f>ROUND(B19*F$16,2)</ns0:f>
       </ns0:c>
       <ns0:c r="G19" s="0">
-        <ns0:f>B19*G$16</ns0:f>
+        <ns0:f>ROUND(B19*G$16,2)</ns0:f>
       </ns0:c>
     </ns0:row>
     <ns0:row r="20">
@@ -444,19 +444,19 @@
         <ns0:v>2.5</ns0:v>
       </ns0:c>
       <ns0:c r="C20" s="0">
-        <ns0:f>B20*C$16</ns0:f>
+        <ns0:f>ROUND(B20*C$16,2)</ns0:f>
       </ns0:c>
       <ns0:c r="D20" s="0">
-        <ns0:f>B20*D$16</ns0:f>
+        <ns0:f>ROUND(B20*D$16,2)</ns0:f>
       </ns0:c>
       <ns0:c r="E20" s="0">
-        <ns0:f>B20*E$16</ns0:f>
+        <ns0:f>ROUND(B20*E$16,2)</ns0:f>
       </ns0:c>
       <ns0:c r="F20" s="0">
-        <ns0:f>B20*F$16</ns0:f>
+        <ns0:f>ROUND(B20*F$16,2)</ns0:f>
       </ns0:c>
       <ns0:c r="G20" s="0">
-        <ns0:f>B20*G$16</ns0:f>
+        <ns0:f>ROUND(B20*G$16,2)</ns0:f>
       </ns0:c>
     </ns0:row>
     <ns0:row r="21">
@@ -469,19 +469,19 @@
         <ns0:v>2.75</ns0:v>
       </ns0:c>
       <ns0:c r="C21" s="0">
-        <ns0:f>B21*C$16</ns0:f>
+        <ns0:f>ROUND(B21*C$16,2)</ns0:f>
       </ns0:c>
       <ns0:c r="D21" s="0">
-        <ns0:f>B21*D$16</ns0:f>
+        <ns0:f>ROUND(B21*D$16,2)</ns0:f>
       </ns0:c>
       <ns0:c r="E21" s="0">
-        <ns0:f>B21*E$16</ns0:f>
+        <ns0:f>ROUND(B21*E$16,2)</ns0:f>
       </ns0:c>
       <ns0:c r="F21" s="0">
-        <ns0:f>B21*F$16</ns0:f>
+        <ns0:f>ROUND(B21*F$16,2)</ns0:f>
       </ns0:c>
       <ns0:c r="G21" s="0">
-        <ns0:f>B21*G$16</ns0:f>
+        <ns0:f>ROUND(B21*G$16,2)</ns0:f>
       </ns0:c>
     </ns0:row>
     <ns0:row r="22">
@@ -494,19 +494,19 @@
         <ns0:v>3.0</ns0:v>
       </ns0:c>
       <ns0:c r="C22" s="0">
-        <ns0:f>B22*C$16</ns0:f>
+        <ns0:f>ROUND(B22*C$16,2)</ns0:f>
       </ns0:c>
       <ns0:c r="D22" s="0">
-        <ns0:f>B22*D$16</ns0:f>
+        <ns0:f>ROUND(B22*D$16,2)</ns0:f>
       </ns0:c>
       <ns0:c r="E22" s="0">
-        <ns0:f>B22*E$16</ns0:f>
+        <ns0:f>ROUND(B22*E$16,2)</ns0:f>
       </ns0:c>
       <ns0:c r="F22" s="0">
-        <ns0:f>B22*F$16</ns0:f>
+        <ns0:f>ROUND(B22*F$16,2)</ns0:f>
       </ns0:c>
       <ns0:c r="G22" s="0">
-        <ns0:f>B22*G$16</ns0:f>
+        <ns0:f>ROUND(B22*G$16,2)</ns0:f>
       </ns0:c>
     </ns0:row>
     <ns0:row r="23">
@@ -519,19 +519,19 @@
         <ns0:v>3.25</ns0:v>
       </ns0:c>
       <ns0:c r="C23" s="0">
-        <ns0:f>B23*C$16</ns0:f>
+        <ns0:f>ROUND(B23*C$16,2)</ns0:f>
       </ns0:c>
       <ns0:c r="D23" s="0">
-        <ns0:f>B23*D$16</ns0:f>
+        <ns0:f>ROUND(B23*D$16,2)</ns0:f>
       </ns0:c>
       <ns0:c r="E23" s="0">
-        <ns0:f>B23*E$16</ns0:f>
+        <ns0:f>ROUND(B23*E$16,2)</ns0:f>
       </ns0:c>
       <ns0:c r="F23" s="0">
-        <ns0:f>B23*F$16</ns0:f>
+        <ns0:f>ROUND(B23*F$16,2)</ns0:f>
       </ns0:c>
       <ns0:c r="G23" s="0">
-        <ns0:f>B23*G$16</ns0:f>
+        <ns0:f>ROUND(B23*G$16,2)</ns0:f>
       </ns0:c>
     </ns0:row>
     <ns0:row r="24">
@@ -544,19 +544,19 @@
         <ns0:v>3.5</ns0:v>
       </ns0:c>
       <ns0:c r="C24" s="0">
-        <ns0:f>B24*C$16</ns0:f>
+        <ns0:f>ROUND(B24*C$16,2)</ns0:f>
       </ns0:c>
       <ns0:c r="D24" s="0">
-        <ns0:f>B24*D$16</ns0:f>
+        <ns0:f>ROUND(B24*D$16,2)</ns0:f>
       </ns0:c>
       <ns0:c r="E24" s="0">
-        <ns0:f>B24*E$16</ns0:f>
+        <ns0:f>ROUND(B24*E$16,2)</ns0:f>
       </ns0:c>
       <ns0:c r="F24" s="0">
-        <ns0:f>B24*F$16</ns0:f>
+        <ns0:f>ROUND(B24*F$16,2)</ns0:f>
       </ns0:c>
       <ns0:c r="G24" s="0">
-        <ns0:f>B24*G$16</ns0:f>
+        <ns0:f>ROUND(B24*G$16,2)</ns0:f>
       </ns0:c>
     </ns0:row>
     <ns0:row r="25"/>
@@ -633,19 +633,19 @@
         <ns0:v>5</ns0:v>
       </ns0:c>
       <ns0:c r="C31" s="0">
-        <ns0:f>B31*C$29</ns0:f>
+        <ns0:f>ROUND(B31*C$29,2)</ns0:f>
       </ns0:c>
       <ns0:c r="D31" s="0">
-        <ns0:f>B31*D$29</ns0:f>
+        <ns0:f>ROUND(B31*D$29,2)</ns0:f>
       </ns0:c>
       <ns0:c r="E31" s="0">
-        <ns0:f>B31*E$29</ns0:f>
+        <ns0:f>ROUND(B31*E$29,2)</ns0:f>
       </ns0:c>
       <ns0:c r="F31" s="0">
-        <ns0:f>B31*F$29</ns0:f>
+        <ns0:f>ROUND(B31*F$29,2)</ns0:f>
       </ns0:c>
       <ns0:c r="G31" s="0">
-        <ns0:f>B31*G$29</ns0:f>
+        <ns0:f>ROUND(B31*G$29,2)</ns0:f>
       </ns0:c>
     </ns0:row>
     <ns0:row r="32">
@@ -658,19 +658,19 @@
         <ns0:v>10</ns0:v>
       </ns0:c>
       <ns0:c r="C32" s="0">
-        <ns0:f>B32*C$29</ns0:f>
+        <ns0:f>ROUND(B32*C$29,2)</ns0:f>
       </ns0:c>
       <ns0:c r="D32" s="0">
-        <ns0:f>B32*D$29</ns0:f>
+        <ns0:f>ROUND(B32*D$29,2)</ns0:f>
       </ns0:c>
       <ns0:c r="E32" s="0">
-        <ns0:f>B32*E$29</ns0:f>
+        <ns0:f>ROUND(B32*E$29,2)</ns0:f>
       </ns0:c>
       <ns0:c r="F32" s="0">
-        <ns0:f>B32*F$29</ns0:f>
+        <ns0:f>ROUND(B32*F$29,2)</ns0:f>
       </ns0:c>
       <ns0:c r="G32" s="0">
-        <ns0:f>B32*G$29</ns0:f>
+        <ns0:f>ROUND(B32*G$29,2)</ns0:f>
       </ns0:c>
     </ns0:row>
     <ns0:row r="33">
@@ -683,19 +683,19 @@
         <ns0:v>10</ns0:v>
       </ns0:c>
       <ns0:c r="C33" s="0">
-        <ns0:f>B33*C$29</ns0:f>
+        <ns0:f>ROUND(B33*C$29,2)</ns0:f>
       </ns0:c>
       <ns0:c r="D33" s="0">
-        <ns0:f>B33*D$29</ns0:f>
+        <ns0:f>ROUND(B33*D$29,2)</ns0:f>
       </ns0:c>
       <ns0:c r="E33" s="0">
-        <ns0:f>B33*E$29</ns0:f>
+        <ns0:f>ROUND(B33*E$29,2)</ns0:f>
       </ns0:c>
       <ns0:c r="F33" s="0">
-        <ns0:f>B33*F$29</ns0:f>
+        <ns0:f>ROUND(B33*F$29,2)</ns0:f>
       </ns0:c>
       <ns0:c r="G33" s="0">
-        <ns0:f>B33*G$29</ns0:f>
+        <ns0:f>ROUND(B33*G$29,2)</ns0:f>
       </ns0:c>
     </ns0:row>
     <ns0:row r="34">
@@ -708,19 +708,19 @@
         <ns0:v>10</ns0:v>
       </ns0:c>
       <ns0:c r="C34" s="0">
-        <ns0:f>B34*C$29</ns0:f>
+        <ns0:f>ROUND(B34*C$29,2)</ns0:f>
       </ns0:c>
       <ns0:c r="D34" s="0">
-        <ns0:f>B34*D$29</ns0:f>
+        <ns0:f>ROUND(B34*D$29,2)</ns0:f>
       </ns0:c>
       <ns0:c r="E34" s="0">
-        <ns0:f>B34*E$29</ns0:f>
+        <ns0:f>ROUND(B34*E$29,2)</ns0:f>
       </ns0:c>
       <ns0:c r="F34" s="0">
-        <ns0:f>B34*F$29</ns0:f>
+        <ns0:f>ROUND(B34*F$29,2)</ns0:f>
       </ns0:c>
       <ns0:c r="G34" s="0">
-        <ns0:f>B34*G$29</ns0:f>
+        <ns0:f>ROUND(B34*G$29,2)</ns0:f>
       </ns0:c>
     </ns0:row>
     <ns0:row r="35">
@@ -733,19 +733,19 @@
         <ns0:v>10</ns0:v>
       </ns0:c>
       <ns0:c r="C35" s="0">
-        <ns0:f>B35*C$29</ns0:f>
+        <ns0:f>ROUND(B35*C$29,2)</ns0:f>
       </ns0:c>
       <ns0:c r="D35" s="0">
-        <ns0:f>B35*D$29</ns0:f>
+        <ns0:f>ROUND(B35*D$29,2)</ns0:f>
       </ns0:c>
       <ns0:c r="E35" s="0">
-        <ns0:f>B35*E$29</ns0:f>
+        <ns0:f>ROUND(B35*E$29,2)</ns0:f>
       </ns0:c>
       <ns0:c r="F35" s="0">
-        <ns0:f>B35*F$29</ns0:f>
+        <ns0:f>ROUND(B35*F$29,2)</ns0:f>
       </ns0:c>
       <ns0:c r="G35" s="0">
-        <ns0:f>B35*G$29</ns0:f>
+        <ns0:f>ROUND(B35*G$29,2)</ns0:f>
       </ns0:c>
     </ns0:row>
     <ns0:row r="36">
@@ -758,19 +758,19 @@
         <ns0:v>20</ns0:v>
       </ns0:c>
       <ns0:c r="C36" s="0">
-        <ns0:f>B36*C$29</ns0:f>
+        <ns0:f>ROUND(B36*C$29,2)</ns0:f>
       </ns0:c>
       <ns0:c r="D36" s="0">
-        <ns0:f>B36*D$29</ns0:f>
+        <ns0:f>ROUND(B36*D$29,2)</ns0:f>
       </ns0:c>
       <ns0:c r="E36" s="0">
-        <ns0:f>B36*E$29</ns0:f>
+        <ns0:f>ROUND(B36*E$29,2)</ns0:f>
       </ns0:c>
       <ns0:c r="F36" s="0">
-        <ns0:f>B36*F$29</ns0:f>
+        <ns0:f>ROUND(B36*F$29,2)</ns0:f>
       </ns0:c>
       <ns0:c r="G36" s="0">
-        <ns0:f>B36*G$29</ns0:f>
+        <ns0:f>ROUND(B36*G$29,2)</ns0:f>
       </ns0:c>
     </ns0:row>
     <ns0:row r="37">
@@ -783,19 +783,19 @@
         <ns0:v>60</ns0:v>
       </ns0:c>
       <ns0:c r="C37" s="0">
-        <ns0:f>B37*C$29</ns0:f>
+        <ns0:f>ROUND(B37*C$29,2)</ns0:f>
       </ns0:c>
       <ns0:c r="D37" s="0">
-        <ns0:f>B37*D$29</ns0:f>
+        <ns0:f>ROUND(B37*D$29,2)</ns0:f>
       </ns0:c>
       <ns0:c r="E37" s="0">
-        <ns0:f>B37*E$29</ns0:f>
+        <ns0:f>ROUND(B37*E$29,2)</ns0:f>
       </ns0:c>
       <ns0:c r="F37" s="0">
-        <ns0:f>B37*F$29</ns0:f>
+        <ns0:f>ROUND(B37*F$29,2)</ns0:f>
       </ns0:c>
       <ns0:c r="G37" s="0">
-        <ns0:f>B37*G$29</ns0:f>
+        <ns0:f>ROUND(B37*G$29,2)</ns0:f>
       </ns0:c>
     </ns0:row>
     <ns0:row r="38"/>
@@ -875,16 +875,16 @@
         <ns0:f>1</ns0:f>
       </ns0:c>
       <ns0:c r="D44" s="0">
-        <ns0:f>MIN(B44*D$42,1)</ns0:f>
+        <ns0:f>ROUND(MIN(B44*D$42,1),2)</ns0:f>
       </ns0:c>
       <ns0:c r="E44" s="0">
-        <ns0:f>MIN(B44*E$42,1)</ns0:f>
+        <ns0:f>ROUND(MIN(B44*E$42,1),2)</ns0:f>
       </ns0:c>
       <ns0:c r="F44" s="0">
-        <ns0:f>MIN(B44*F$42,1)</ns0:f>
+        <ns0:f>ROUND(MIN(B44*F$42,1),2)</ns0:f>
       </ns0:c>
       <ns0:c r="G44" s="0">
-        <ns0:f>MIN(B44*G$42,1)</ns0:f>
+        <ns0:f>ROUND(MIN(B44*G$42,1),2)</ns0:f>
       </ns0:c>
     </ns0:row>
     <ns0:row r="45">
@@ -900,16 +900,16 @@
         <ns0:f>1</ns0:f>
       </ns0:c>
       <ns0:c r="D45" s="0">
-        <ns0:f>MIN(B45*D$42,1)</ns0:f>
+        <ns0:f>ROUND(MIN(B45*D$42,1),2)</ns0:f>
       </ns0:c>
       <ns0:c r="E45" s="0">
-        <ns0:f>MIN(B45*E$42,1)</ns0:f>
+        <ns0:f>ROUND(MIN(B45*E$42,1),2)</ns0:f>
       </ns0:c>
       <ns0:c r="F45" s="0">
-        <ns0:f>MIN(B45*F$42,1)</ns0:f>
+        <ns0:f>ROUND(MIN(B45*F$42,1),2)</ns0:f>
       </ns0:c>
       <ns0:c r="G45" s="0">
-        <ns0:f>MIN(B45*G$42,1)</ns0:f>
+        <ns0:f>ROUND(MIN(B45*G$42,1),2)</ns0:f>
       </ns0:c>
     </ns0:row>
     <ns0:row r="46">
@@ -925,16 +925,16 @@
         <ns0:f>1</ns0:f>
       </ns0:c>
       <ns0:c r="D46" s="0">
-        <ns0:f>MIN(B46*D$42,1)</ns0:f>
+        <ns0:f>ROUND(MIN(B46*D$42,1),2)</ns0:f>
       </ns0:c>
       <ns0:c r="E46" s="0">
-        <ns0:f>MIN(B46*E$42,1)</ns0:f>
+        <ns0:f>ROUND(MIN(B46*E$42,1),2)</ns0:f>
       </ns0:c>
       <ns0:c r="F46" s="0">
-        <ns0:f>MIN(B46*F$42,1)</ns0:f>
+        <ns0:f>ROUND(MIN(B46*F$42,1),2)</ns0:f>
       </ns0:c>
       <ns0:c r="G46" s="0">
-        <ns0:f>MIN(B46*G$42,1)</ns0:f>
+        <ns0:f>ROUND(MIN(B46*G$42,1),2)</ns0:f>
       </ns0:c>
     </ns0:row>
     <ns0:row r="47">
@@ -950,16 +950,16 @@
         <ns0:f>1</ns0:f>
       </ns0:c>
       <ns0:c r="D47" s="0">
-        <ns0:f>MIN(B47*D$42,1)</ns0:f>
+        <ns0:f>ROUND(MIN(B47*D$42,1),2)</ns0:f>
       </ns0:c>
       <ns0:c r="E47" s="0">
-        <ns0:f>MIN(B47*E$42,1)</ns0:f>
+        <ns0:f>ROUND(MIN(B47*E$42,1),2)</ns0:f>
       </ns0:c>
       <ns0:c r="F47" s="0">
-        <ns0:f>MIN(B47*F$42,1)</ns0:f>
+        <ns0:f>ROUND(MIN(B47*F$42,1),2)</ns0:f>
       </ns0:c>
       <ns0:c r="G47" s="0">
-        <ns0:f>MIN(B47*G$42,1)</ns0:f>
+        <ns0:f>ROUND(MIN(B47*G$42,1),2)</ns0:f>
       </ns0:c>
     </ns0:row>
     <ns0:row r="48">
@@ -975,16 +975,16 @@
         <ns0:f>1</ns0:f>
       </ns0:c>
       <ns0:c r="D48" s="0">
-        <ns0:f>MIN(B48*D$42,1)</ns0:f>
+        <ns0:f>ROUND(MIN(B48*D$42,1),2)</ns0:f>
       </ns0:c>
       <ns0:c r="E48" s="0">
-        <ns0:f>MIN(B48*E$42,1)</ns0:f>
+        <ns0:f>ROUND(MIN(B48*E$42,1),2)</ns0:f>
       </ns0:c>
       <ns0:c r="F48" s="0">
-        <ns0:f>MIN(B48*F$42,1)</ns0:f>
+        <ns0:f>ROUND(MIN(B48*F$42,1),2)</ns0:f>
       </ns0:c>
       <ns0:c r="G48" s="0">
-        <ns0:f>MIN(B48*G$42,1)</ns0:f>
+        <ns0:f>ROUND(MIN(B48*G$42,1),2)</ns0:f>
       </ns0:c>
     </ns0:row>
     <ns0:row r="49">
@@ -1000,16 +1000,16 @@
         <ns0:f>1</ns0:f>
       </ns0:c>
       <ns0:c r="D49" s="0">
-        <ns0:f>MIN(B49*D$42,1)</ns0:f>
+        <ns0:f>ROUND(MIN(B49*D$42,1),2)</ns0:f>
       </ns0:c>
       <ns0:c r="E49" s="0">
-        <ns0:f>MIN(B49*E$42,1)</ns0:f>
+        <ns0:f>ROUND(MIN(B49*E$42,1),2)</ns0:f>
       </ns0:c>
       <ns0:c r="F49" s="0">
-        <ns0:f>MIN(B49*F$42,1)</ns0:f>
+        <ns0:f>ROUND(MIN(B49*F$42,1),2)</ns0:f>
       </ns0:c>
       <ns0:c r="G49" s="0">
-        <ns0:f>MIN(B49*G$42,1)</ns0:f>
+        <ns0:f>ROUND(MIN(B49*G$42,1),2)</ns0:f>
       </ns0:c>
     </ns0:row>
     <ns0:row r="50">
@@ -1025,16 +1025,16 @@
         <ns0:f>1</ns0:f>
       </ns0:c>
       <ns0:c r="D50" s="0">
-        <ns0:f>MIN(B50*D$42,1)</ns0:f>
+        <ns0:f>ROUND(MIN(B50*D$42,1),2)</ns0:f>
       </ns0:c>
       <ns0:c r="E50" s="0">
-        <ns0:f>MIN(B50*E$42,1)</ns0:f>
+        <ns0:f>ROUND(MIN(B50*E$42,1),2)</ns0:f>
       </ns0:c>
       <ns0:c r="F50" s="0">
-        <ns0:f>MIN(B50*F$42,1)</ns0:f>
+        <ns0:f>ROUND(MIN(B50*F$42,1),2)</ns0:f>
       </ns0:c>
       <ns0:c r="G50" s="0">
-        <ns0:f>MIN(B50*G$42,1)</ns0:f>
+        <ns0:f>ROUND(MIN(B50*G$42,1),2)</ns0:f>
       </ns0:c>
     </ns0:row>
     <ns0:row r="51"/>

</xml_diff>

<commit_message>
Sync preset values with updated Presets.xlsx
Updated values from Presets.xlsx:
- Intensity multipliers: Subtle 1.5x, Dramatic 0.8x, Cinematic 0.5x, Epic 0.3x
- Duration multipliers: Very Short 0.35x, Long 1.35x, Extended 1.7x
- Dismemberment chance: 30% (was 60%)
- Last Enemy cooldown: 30s (was 20s)
- Last Stand: timeScale 0.30 (was 0.21), duration 4s (was 3.5s), cooldown 90s (was 60s)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Presets.xlsx
+++ b/Presets.xlsx
@@ -93,19 +93,19 @@
     <ns0:row r="2"/>
     <ns0:row r="3">
       <ns0:c r="C3" s="0">
-        <ns0:v>1.35</ns0:v>
+        <ns0:v>1.5</ns0:v>
       </ns0:c>
       <ns0:c r="D3" s="0">
         <ns0:v>1.0</ns0:v>
       </ns0:c>
       <ns0:c r="E3" s="0">
-        <ns0:v>0.85</ns0:v>
+        <ns0:v>0.8</ns0:v>
       </ns0:c>
       <ns0:c r="F3" s="0">
-        <ns0:v>0.7</ns0:v>
+        <ns0:v>0.5</ns0:v>
       </ns0:c>
       <ns0:c r="G3" s="0">
-        <ns0:v>0.55</ns0:v>
+        <ns0:v>0.3</ns0:v>
       </ns0:c>
     </ns0:row>
     <ns0:row r="4">
@@ -302,7 +302,7 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="B11" s="0">
-        <ns0:v>0.21</ns0:v>
+        <ns0:v>0.3</ns0:v>
       </ns0:c>
       <ns0:c r="C11" s="0">
         <ns0:f>ROUND(B11*C$3,2)</ns0:f>
@@ -332,7 +332,7 @@
     <ns0:row r="15"/>
     <ns0:row r="16">
       <ns0:c r="C16" s="0">
-        <ns0:v>0.5</ns0:v>
+        <ns0:v>0.35</ns0:v>
       </ns0:c>
       <ns0:c r="D16" s="0">
         <ns0:v>0.7</ns0:v>
@@ -341,10 +341,10 @@
         <ns0:v>1.0</ns0:v>
       </ns0:c>
       <ns0:c r="F16" s="0">
-        <ns0:v>1.3</ns0:v>
+        <ns0:v>1.35</ns0:v>
       </ns0:c>
       <ns0:c r="G16" s="0">
-        <ns0:v>1.5</ns0:v>
+        <ns0:v>1.7</ns0:v>
       </ns0:c>
     </ns0:row>
     <ns0:row r="17">
@@ -541,7 +541,7 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="B24" s="0">
-        <ns0:v>3.5</ns0:v>
+        <ns0:v>4.0</ns0:v>
       </ns0:c>
       <ns0:c r="C24" s="0">
         <ns0:f>ROUND(B24*C$16,2)</ns0:f>
@@ -755,7 +755,7 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="B36" s="0">
-        <ns0:v>20</ns0:v>
+        <ns0:v>30</ns0:v>
       </ns0:c>
       <ns0:c r="C36" s="0">
         <ns0:f>ROUND(B36*C$29,2)</ns0:f>
@@ -780,7 +780,7 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="B37" s="0">
-        <ns0:v>60</ns0:v>
+        <ns0:v>90</ns0:v>
       </ns0:c>
       <ns0:c r="C37" s="0">
         <ns0:f>ROUND(B37*C$29,2)</ns0:f>
@@ -919,7 +919,7 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="B46" s="0">
-        <ns0:v>0.6</ns0:v>
+        <ns0:v>0.3</ns0:v>
       </ns0:c>
       <ns0:c r="C46" s="0">
         <ns0:f>1</ns0:f>

</xml_diff>